<commit_message>
Done lab 5 and lab 5+
</commit_message>
<xml_diff>
--- a/lab2/wykresy_NAI.xlsx
+++ b/lab2/wykresy_NAI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patry\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F794CC-F52C-45B2-8694-0D4E73684EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA01DF43-0C74-4D9C-BF8E-8EB8C8A851B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EA52211D-3F7D-46BD-B3D5-A2C5212B87A0}"/>
   </bookViews>
@@ -36,72 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Beale function</t>
-  </si>
-  <si>
-    <t>MatyasFunction</t>
   </si>
   <si>
     <t>BoothFunction</t>
   </si>
   <si>
-    <t>1.18937</t>
-  </si>
-  <si>
-    <t>36.019</t>
-  </si>
-  <si>
-    <t>4.33336</t>
-  </si>
-  <si>
-    <t>0.324868</t>
-  </si>
-  <si>
-    <t>0.0388347</t>
-  </si>
-  <si>
-    <t>0.00346079</t>
-  </si>
-  <si>
-    <t>0.000423632</t>
-  </si>
-  <si>
-    <t>0.00000972846</t>
-  </si>
-  <si>
-    <t>0.0000687554</t>
-  </si>
-  <si>
-    <t>0.000737593</t>
-  </si>
-  <si>
-    <t>0.00987842</t>
-  </si>
-  <si>
-    <t>0.0876569</t>
-  </si>
-  <si>
-    <t>11.0426</t>
-  </si>
-  <si>
-    <t>0.61308</t>
-  </si>
-  <si>
-    <t>0.0476098</t>
-  </si>
-  <si>
-    <t>0.00581067</t>
-  </si>
-  <si>
-    <t>0.00037757</t>
-  </si>
-  <si>
-    <t>0.000057816</t>
-  </si>
-  <si>
-    <t>Iterations</t>
+    <t>MatyasFunction</t>
   </si>
 </sst>
 </file>
@@ -139,7 +82,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -147,44 +90,20 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
@@ -269,7 +188,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$G$1</c:f>
+              <c:f>Arkusz1!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -290,7 +209,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Arkusz1!$F$2:$F$7</c:f>
+              <c:f>Arkusz1!$A$2:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -317,27 +236,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$G$2:$G$7</c:f>
+              <c:f>Arkusz1!$B$2:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>0.0000000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>11.471299999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.75148499999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>5.4472E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>3.91896E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2.8396900000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>6.2768000000000002E-7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -582,6 +501,9 @@
               <c:f>Arkusz1!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BoothFunction</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -597,7 +519,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Arkusz1!$F$2:$F$7</c:f>
+              <c:f>Arkusz1!$A$2:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -624,27 +546,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$H$2:$H$7</c:f>
+              <c:f>Arkusz1!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>0.0000000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>36.018999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4.3333599999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.32486799999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>3.88347E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>3.46079E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>4.2363200000000001E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -678,7 +600,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Arkusz1!$G$1</c15:sqref>
+                          <c15:sqref>Arkusz1!$B$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -705,7 +627,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Arkusz1!$F$2:$F$7</c15:sqref>
+                          <c15:sqref>Arkusz1!$A$2:$A$7</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -738,7 +660,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Arkusz1!$G$2:$G$7</c15:sqref>
+                          <c15:sqref>Arkusz1!$B$2:$B$7</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -746,22 +668,22 @@
                       <c:formatCode>0.0000000</c:formatCode>
                       <c:ptCount val="6"/>
                       <c:pt idx="0">
-                        <c:v>0</c:v>
+                        <c:v>11.471299999999999</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0</c:v>
+                        <c:v>0.75148499999999996</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0</c:v>
+                        <c:v>5.4472E-2</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0</c:v>
+                        <c:v>3.91896E-3</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>0</c:v>
+                        <c:v>2.8396900000000002E-4</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>0</c:v>
+                        <c:v>6.2768000000000002E-7</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1028,6 +950,9 @@
               <c:f>Arkusz1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MatyasFunction</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -1043,7 +968,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Arkusz1!$F$2:$F$7</c:f>
+              <c:f>Arkusz1!$A$2:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1070,27 +995,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$I$2:$I$7</c:f>
+              <c:f>Arkusz1!$D$2:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>0.0000000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1.18937</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>8.7656899999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>9.8784200000000006E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>7.3759300000000004E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>6.8755400000000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>9.7284600000000007E-6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1124,7 +1049,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Arkusz1!$G$1</c15:sqref>
+                          <c15:sqref>Arkusz1!$B$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1151,7 +1076,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Arkusz1!$F$2:$F$7</c15:sqref>
+                          <c15:sqref>Arkusz1!$A$2:$A$7</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1184,7 +1109,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Arkusz1!$G$2:$G$7</c15:sqref>
+                          <c15:sqref>Arkusz1!$B$2:$B$7</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1192,22 +1117,22 @@
                       <c:formatCode>0.0000000</c:formatCode>
                       <c:ptCount val="6"/>
                       <c:pt idx="0">
-                        <c:v>0</c:v>
+                        <c:v>11.471299999999999</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0</c:v>
+                        <c:v>0.75148499999999996</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0</c:v>
+                        <c:v>5.4472E-2</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0</c:v>
+                        <c:v>3.91896E-3</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>0</c:v>
+                        <c:v>2.8396900000000002E-4</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>0</c:v>
+                        <c:v>6.2768000000000002E-7</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1234,6 +1159,9 @@
                     </c:extLst>
                     <c:strCache>
                       <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>BoothFunction</c:v>
+                      </c:pt>
                     </c:strCache>
                   </c:strRef>
                 </c:tx>
@@ -1252,7 +1180,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Arkusz1!$F$2:$F$7</c15:sqref>
+                          <c15:sqref>Arkusz1!$A$2:$A$7</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1285,7 +1213,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Arkusz1!$H$2:$H$7</c15:sqref>
+                          <c15:sqref>Arkusz1!$C$2:$C$7</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1293,22 +1221,22 @@
                       <c:formatCode>0.0000000</c:formatCode>
                       <c:ptCount val="6"/>
                       <c:pt idx="0">
-                        <c:v>0</c:v>
+                        <c:v>36.018999999999998</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0</c:v>
+                        <c:v>4.3333599999999999</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0</c:v>
+                        <c:v>0.32486799999999999</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0</c:v>
+                        <c:v>3.88347E-2</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>0</c:v>
+                        <c:v>3.46079E-3</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>0</c:v>
+                        <c:v>4.2363200000000001E-4</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3176,15 +3104,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
+      <xdr:colOff>742949</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
+      <xdr:colOff>571499</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3212,15 +3140,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3545,163 +3473,158 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D2F22A6-FE40-4ABF-A969-653AE801B9D0}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" customWidth="1"/>
-    <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="F1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="7" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E2" s="4"/>
-      <c r="F2" s="6">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>10</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>15</v>
+      <c r="B2" s="5">
+        <v>11.471299999999999</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>4</v>
+      <c r="C2" s="5">
+        <v>36.018999999999998</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>3</v>
+      <c r="D2" s="5">
+        <v>1.18937</v>
       </c>
+      <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E3" s="4"/>
-      <c r="F3" s="6">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>100</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>16</v>
+      <c r="B3" s="5">
+        <v>0.75148499999999996</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>5</v>
+      <c r="C3" s="5">
+        <v>4.3333599999999999</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>14</v>
+      <c r="D3" s="5">
+        <v>8.7656899999999996E-2</v>
       </c>
+      <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E4" s="4"/>
-      <c r="F4" s="6">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>1000</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>17</v>
+      <c r="B4" s="5">
+        <v>5.4472E-2</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>6</v>
+      <c r="C4" s="5">
+        <v>0.32486799999999999</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>13</v>
+      <c r="D4" s="5">
+        <v>9.8784200000000006E-3</v>
       </c>
+      <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E5" s="4"/>
-      <c r="F5" s="6">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>10000</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>18</v>
+      <c r="B5" s="5">
+        <v>3.91896E-3</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>7</v>
+      <c r="C5" s="5">
+        <v>3.88347E-2</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>12</v>
+      <c r="D5" s="5">
+        <v>7.3759300000000004E-4</v>
       </c>
+      <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E6" s="4"/>
-      <c r="F6" s="6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>100000</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>19</v>
+      <c r="B6" s="5">
+        <v>2.8396900000000002E-4</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>8</v>
+      <c r="C6" s="5">
+        <v>3.46079E-3</v>
       </c>
-      <c r="I6" s="8" t="s">
-        <v>11</v>
+      <c r="D6" s="5">
+        <v>6.8755400000000002E-5</v>
       </c>
+      <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E7" s="4"/>
-      <c r="F7" s="6">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>1000000</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>20</v>
+      <c r="B7" s="5">
+        <v>6.2768000000000002E-7</v>
       </c>
-      <c r="H7" s="8" t="s">
-        <v>9</v>
+      <c r="C7" s="5">
+        <v>4.2363200000000001E-4</v>
       </c>
-      <c r="I7" s="8" t="s">
-        <v>10</v>
+      <c r="D7" s="5">
+        <v>9.7284600000000007E-6</v>
       </c>
+      <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
+      <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
+      <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
+      <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
+      <c r="B13" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1" tooltip="Goldstein–Price function (page does not exist)" display="https://en.wikipedia.org/w/index.php?title=Goldstein%E2%80%93Price_function&amp;action=edit&amp;redlink=1" xr:uid="{892AAE3E-E893-4011-909B-313605DCE74C}"/>
+    <hyperlink ref="D1" r:id="rId2" tooltip="Booth function (page does not exist)" display="https://en.wikipedia.org/w/index.php?title=Booth_function&amp;action=edit&amp;redlink=1" xr:uid="{BDE26731-A3DE-4DCE-A240-182F870628C5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>